<commit_message>
finished review and diagram
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="141">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Popescu Ionel</t>
   </si>
   <si>
-    <t>Georgescu Anca</t>
-  </si>
-  <si>
     <t>Requirements Document</t>
   </si>
   <si>
@@ -250,44 +247,237 @@
     <t>Nu exista un sistem coerent de tratare a erorilor.</t>
   </si>
   <si>
-    <t>Arhitectura MVC si Observer( prin lutilizarea ObservableList)</t>
-  </si>
-  <si>
     <t>TaskIO</t>
   </si>
   <si>
-    <t>Arhitectura este de tipul Modev-View-Controller, clar definita pentru entitea Task, dar lipseste repositoryul si validatorul cu desavarsire.</t>
-  </si>
-  <si>
-    <t>TaskIO s-ar putea redenumi TaskFileHandler.</t>
-  </si>
-  <si>
     <t>TaskService</t>
   </si>
   <si>
     <t>Functia fromTimeUnit ar trebui mutatata in DateService.</t>
   </si>
   <si>
-    <t>Nu, numele rolurilor din agregări și asocieri nu descriu întotdeauna corect relațiile dintre clasele respective.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conform diagramei, clasele ArrayTaskList si LinkedList indeplinesc aceeasi functie, ar fi necesar eliminarea uneia pentru a evita redundanta.  </t>
-  </si>
-  <si>
     <t>Clasele si si relatiile dintre ele sunt consistente in raport cu cerintele.</t>
+  </si>
+  <si>
+    <t>Copas Codrut</t>
+  </si>
+  <si>
+    <t>Cosma Tudor</t>
+  </si>
+  <si>
+    <t>Arhitectura este de tipul Modev-View-Controller, clar definita pentru entitea Task, dar lipseste repository si validatorul.</t>
+  </si>
+  <si>
+    <t>Partitionarea in pachete este consistenta cu pattern-ul MVC.</t>
+  </si>
+  <si>
+    <t>Denumirea TaskIO este ambigua. Ar putea fi redenumita TaskFileHandler pentru a reflecta mai bine responsabilitatea clasei</t>
+  </si>
+  <si>
+    <t>Notificator</t>
+  </si>
+  <si>
+    <t>Denumirea de Notificator duce cu gandul la un concept abstract, iar ea este de fapt o concretizare. Ar trebui denumit TaskNotifier.</t>
+  </si>
+  <si>
+    <t>Nu, numele rolurilor din agregări și asocieri nu descriu întotdeauna corect relațiile dintre clasele respective, uneori creand confuzie.</t>
+  </si>
+  <si>
+    <t>TaskService/Controller</t>
+  </si>
+  <si>
+    <t>Arhitectura MVC, Observer( prin utilizarea ObservableList din JAVAFX) si Strategy(ArrayTaskList si LinkedTaskList)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TasksOperations nu ar trebui sa fie in pachetul model. Mai degraba in Service. </t>
+  </si>
+  <si>
+    <t>model package</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>NewEditController</t>
+  </si>
+  <si>
+    <t>Nu se verifica pentru non-repeating tasks daca before &lt; after</t>
+  </si>
+  <si>
+    <t>TaskIO(87/73)</t>
+  </si>
+  <si>
+    <t>Posibila folosirea try-with-resources in loc de finally</t>
+  </si>
+  <si>
+    <t>TaslkIO</t>
+  </si>
+  <si>
+    <t>Nu toate erorile posibile la citire/scriere nu sunt handle-uite, lipsin catch statements</t>
+  </si>
+  <si>
+    <t>Se folosesc ca tipuri clase concrete in loc de abstractizari</t>
+  </si>
+  <si>
+    <t>TasksOperations(8)</t>
+  </si>
+  <si>
+    <t>TaskList/TasksOperations</t>
+  </si>
+  <si>
+    <t>Metoda incoming este definita de 2 ori, dar doar o implementare este folosita.</t>
+  </si>
+  <si>
+    <t>Avem un singur branch.</t>
+  </si>
+  <si>
+    <t>Task/107</t>
+  </si>
+  <si>
+    <t>Interval poate fi 0.</t>
+  </si>
+  <si>
+    <t>TaskIo/103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write scrie taskuril cu ; sau . la sfarsit. Read nu tine cont de asta  </t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>TaskIO/50</t>
+  </si>
+  <si>
+    <t>titleLength  nu este folosit</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>TaskIO/178</t>
+  </si>
+  <si>
+    <t>Utilizarea numelor de variabile i si j prodcue confuzie si nu sunt sugestive.</t>
+  </si>
+  <si>
+    <t>NewEditController,85</t>
+  </si>
+  <si>
+    <t>No default case for switch</t>
+  </si>
+  <si>
+    <t>switch fara metoda default</t>
+  </si>
+  <si>
+    <t>metoda default arunca IllegalStateException</t>
+  </si>
+  <si>
+    <t>NewEditController,201</t>
+  </si>
+  <si>
+    <t>Utilizat sout ca loggersout result</t>
+  </si>
+  <si>
+    <t>log result</t>
+  </si>
+  <si>
+    <t>Notificator,41</t>
+  </si>
+  <si>
+    <t>Two if clauses</t>
+  </si>
+  <si>
+    <t>Merged the if clauses into one</t>
+  </si>
+  <si>
+    <t>Notificator,59</t>
+  </si>
+  <si>
+    <t>Useless Curly Braces</t>
+  </si>
+  <si>
+    <t>Curly Braces</t>
+  </si>
+  <si>
+    <t>Lambda Function</t>
+  </si>
+  <si>
+    <t>ArrayTaskList,Task</t>
+  </si>
+  <si>
+    <t>Clone constructor</t>
+  </si>
+  <si>
+    <t>Cloneable Interface</t>
+  </si>
+  <si>
+    <t>Unnecesssary complexity</t>
+  </si>
+  <si>
+    <t>Task,106</t>
+  </si>
+  <si>
+    <t>Complex Method</t>
+  </si>
+  <si>
+    <t>Single complex function</t>
+  </si>
+  <si>
+    <t>Nu pare ca taskService contine metode pentru editare/stergere, acestea fiind facute direct in Controller(logic ar fi Controller -&gt; Service -&gt; IO operations)(nice to have)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -378,6 +568,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -480,86 +677,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,6 +774,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>79527</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>86402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE36DF02-CC07-A70B-0CA3-A137B909A3B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8125558" y="5912827"/>
+          <a:ext cx="8087854" cy="4848902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -870,15 +1117,15 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
@@ -891,33 +1138,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="H1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="J3" s="17">
         <v>232</v>
@@ -927,15 +1174,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="27"/>
+      <c r="D4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="38" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="J4" s="3">
         <v>232</v>
@@ -945,15 +1192,15 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="29"/>
+      <c r="D5" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="J5" s="3">
         <v>232</v>
@@ -964,19 +1211,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="24"/>
+      <c r="D6" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="26">
         <v>45811</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -997,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1012,13 +1259,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1027,13 +1274,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1042,13 +1289,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1057,13 +1304,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1072,13 +1319,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1087,13 +1334,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -1102,13 +1349,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1116,14 +1363,14 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -1131,14 +1378,14 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="39" t="s">
+      <c r="C19" s="23" t="s">
         <v>53</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1146,14 +1393,14 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>55</v>
+      <c r="C20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -1229,15 +1476,15 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="22.109375" style="6" customWidth="1"/>
@@ -1249,33 +1496,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="H1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="J3" s="17">
         <v>232</v>
@@ -1285,15 +1532,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="30"/>
+      <c r="D4" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3">
         <v>232</v>
@@ -1303,15 +1550,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="32"/>
+      <c r="D5" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="3">
         <v>232</v>
@@ -1322,15 +1569,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="26">
+        <v>45811</v>
+      </c>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1351,43 +1602,43 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1396,13 +1647,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1411,13 +1662,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1426,101 +1677,119 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="E18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
@@ -1529,7 +1798,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
@@ -1576,6 +1845,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1586,19 +1856,19 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
@@ -1607,30 +1877,30 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="H1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -1639,12 +1909,12 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="33"/>
+      <c r="D4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1653,12 +1923,12 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1668,15 +1938,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1692,112 +1962,182 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
@@ -1896,6 +2236,7 @@
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="D5:E5"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1908,20 +2249,20 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
@@ -1930,33 +2271,33 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="H1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="17">
         <v>232</v>
@@ -1964,15 +2305,15 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+        <v>23</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="3">
         <v>232</v>
@@ -1982,13 +2323,13 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" s="3">
         <v>232</v>
@@ -1999,8 +2340,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2008,75 +2349,119 @@
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F11" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2230,11 +2615,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="C32" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="18"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.3">

</xml_diff>